<commit_message>
Consultas de Multiplas Tabelas e Pivot
</commit_message>
<xml_diff>
--- a/ExcelData/ProcedimentosData.xlsx
+++ b/ExcelData/ProcedimentosData.xlsx
@@ -125,11 +125,12 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9">
-  <numFmts count="4">
+  <numFmts count="5">
     <numFmt numFmtId="176" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="177" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="178" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="179" formatCode="_-&quot;R$&quot;\ * #,##0_-;\-&quot;R$&quot;\ * #,##0_-;_-&quot;R$&quot;\ * &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="180" formatCode="0.00_);[Red]\(0.00\)"/>
   </numFmts>
   <fonts count="23">
     <font>
@@ -751,10 +752,11 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="180" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="49">
@@ -1078,7 +1080,7 @@
   <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="D2" sqref="D2:D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="4"/>
@@ -1086,7 +1088,7 @@
     <col min="1" max="1" width="16.2857142857143" customWidth="1"/>
     <col min="2" max="2" width="128.714285714286" customWidth="1"/>
     <col min="3" max="3" width="11" customWidth="1"/>
-    <col min="4" max="4" width="9.28571428571429"/>
+    <col min="4" max="4" width="12.5714285714286"/>
     <col min="5" max="5" width="12.4285714285714" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1117,10 +1119,10 @@
       <c r="C2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="1">
-        <v>134.5</v>
-      </c>
-      <c r="E2" s="3" t="s">
+      <c r="D2" s="3">
+        <v>482.56</v>
+      </c>
+      <c r="E2" s="4" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1134,10 +1136,10 @@
       <c r="C3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="1">
-        <v>187.2</v>
-      </c>
-      <c r="E3" s="3" t="s">
+      <c r="D3" s="3">
+        <v>713.21</v>
+      </c>
+      <c r="E3" s="4" t="s">
         <v>10</v>
       </c>
     </row>
@@ -1151,10 +1153,10 @@
       <c r="C4" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="1">
-        <v>112.8</v>
-      </c>
-      <c r="E4" s="3" t="s">
+      <c r="D4" s="3">
+        <v>619.88</v>
+      </c>
+      <c r="E4" s="4" t="s">
         <v>13</v>
       </c>
     </row>
@@ -1168,10 +1170,10 @@
       <c r="C5" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="1">
-        <v>156.7</v>
-      </c>
-      <c r="E5" s="3" t="s">
+      <c r="D5" s="3">
+        <v>347.45</v>
+      </c>
+      <c r="E5" s="4" t="s">
         <v>15</v>
       </c>
     </row>
@@ -1185,10 +1187,10 @@
       <c r="C6" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D6" s="1">
-        <v>103.4</v>
-      </c>
-      <c r="E6" s="3" t="s">
+      <c r="D6" s="3">
+        <v>890.33</v>
+      </c>
+      <c r="E6" s="4" t="s">
         <v>17</v>
       </c>
     </row>
@@ -1202,10 +1204,10 @@
       <c r="C7" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D7" s="1">
-        <v>121.9</v>
-      </c>
-      <c r="E7" s="3" t="s">
+      <c r="D7" s="3">
+        <v>250.7</v>
+      </c>
+      <c r="E7" s="4" t="s">
         <v>19</v>
       </c>
     </row>
@@ -1219,10 +1221,10 @@
       <c r="C8" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D8" s="1">
-        <v>198.6</v>
-      </c>
-      <c r="E8" s="3" t="s">
+      <c r="D8" s="3">
+        <v>670.12</v>
+      </c>
+      <c r="E8" s="4" t="s">
         <v>21</v>
       </c>
     </row>
@@ -1236,10 +1238,10 @@
       <c r="C9" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D9" s="1">
-        <v>143.75</v>
-      </c>
-      <c r="E9" s="3" t="s">
+      <c r="D9" s="3">
+        <v>480.94</v>
+      </c>
+      <c r="E9" s="4" t="s">
         <v>23</v>
       </c>
     </row>
@@ -1253,10 +1255,10 @@
       <c r="C10" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D10" s="1">
-        <v>172.3</v>
-      </c>
-      <c r="E10" s="3" t="s">
+      <c r="D10" s="3">
+        <v>790.27</v>
+      </c>
+      <c r="E10" s="4" t="s">
         <v>25</v>
       </c>
     </row>
@@ -1270,10 +1272,10 @@
       <c r="C11" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D11" s="1">
-        <v>115.25</v>
-      </c>
-      <c r="E11" s="3" t="s">
+      <c r="D11" s="3">
+        <v>550.61</v>
+      </c>
+      <c r="E11" s="4" t="s">
         <v>26</v>
       </c>
     </row>
@@ -1287,10 +1289,10 @@
       <c r="C12" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D12" s="1">
-        <v>129.8</v>
-      </c>
-      <c r="E12" s="3" t="s">
+      <c r="D12" s="3">
+        <v>930.18</v>
+      </c>
+      <c r="E12" s="4" t="s">
         <v>28</v>
       </c>
     </row>
@@ -1304,10 +1306,10 @@
       <c r="C13" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D13" s="1">
-        <v>106.5</v>
-      </c>
-      <c r="E13" s="3" t="s">
+      <c r="D13" s="3">
+        <v>360.75</v>
+      </c>
+      <c r="E13" s="4" t="s">
         <v>30</v>
       </c>
     </row>
@@ -1321,10 +1323,10 @@
       <c r="C14" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D14" s="1">
-        <v>163.4</v>
-      </c>
-      <c r="E14" s="3" t="s">
+      <c r="D14" s="3">
+        <v>630.49</v>
+      </c>
+      <c r="E14" s="4" t="s">
         <v>32</v>
       </c>
     </row>
@@ -1338,10 +1340,10 @@
       <c r="C15" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D15" s="1">
-        <v>190.2</v>
-      </c>
-      <c r="E15" s="3" t="s">
+      <c r="D15" s="3">
+        <v>800.02</v>
+      </c>
+      <c r="E15" s="4" t="s">
         <v>34</v>
       </c>
     </row>

</xml_diff>